<commit_message>
Add items to GS Summary Table
</commit_message>
<xml_diff>
--- a/GenericScenarioEvaluation/output.xlsx
+++ b/GenericScenarioEvaluation/output.xlsx
@@ -2,22 +2,22 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Generic Scenarios" sheetId="1" r:id="R43e6e30d3934413d"/>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Process Descriptions" sheetId="2" r:id="Rf6c298564e374745"/>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Occupational Exposure" sheetId="3" r:id="R8140cb9365fb4582"/>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Environmental Releases" sheetId="4" r:id="Rd6911d36456f48dd"/>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ProductionRate" sheetId="5" r:id="R0f1c669406fa4d51"/>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Control Technologies" sheetId="6" r:id="R4985b052f5934cf8"/>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Calculations" sheetId="7" r:id="Rae1d24ec912041b6"/>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Concntrations" sheetId="8" r:id="Rf9898f1226cb4013"/>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Number of Sites" sheetId="9" r:id="R0b5be3094b9f4ed6"/>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Operating Days" sheetId="10" r:id="R782aefd8a2b54384"/>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Workers" sheetId="11" r:id="R481dae75f9d34b9c"/>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Shifts" sheetId="12" r:id="R4803935ed6e343a2"/>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PPE" sheetId="13" r:id="R8529c3bb1df74fa1"/>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Use Rates" sheetId="14" r:id="R2021a7c96f1a405a"/>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Parameters" sheetId="15" r:id="R970a2cb67ca44669"/>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Data Values" sheetId="16" r:id="R9106308d71a440fa"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Generic Scenarios" sheetId="1" r:id="Rae6a134503af45a3"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Process Descriptions" sheetId="2" r:id="Rcdebf2ab46dd4a73"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Occupational Exposure" sheetId="3" r:id="Ra65d249bd44d450c"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Environmental Releases" sheetId="4" r:id="R616a6b0641ac4c0d"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ProductionRate" sheetId="5" r:id="R31199754392c494a"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Control Technologies" sheetId="6" r:id="R87a31ca16a564f8c"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Calculations" sheetId="7" r:id="Rdcedf07392804834"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Concntrations" sheetId="8" r:id="Ra9ba511d1d114744"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Number of Sites" sheetId="9" r:id="R0ba167bd99634742"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Operating Days" sheetId="10" r:id="R8b21d71effcd4e4c"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Workers" sheetId="11" r:id="R50bc188c28f94040"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Shifts" sheetId="12" r:id="Rd18d94e5a7954896"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PPE" sheetId="13" r:id="R4f2a4bcefa1c4e81"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Use Rates" sheetId="14" r:id="Rc917a07d02d14b46"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Parameters" sheetId="15" r:id="R993fa95db6d94409"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Data Values" sheetId="16" r:id="R03c35178f6f943bc"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -36,6 +36,24 @@
         <x:v>Developed By</x:v>
       </x:c>
       <x:c t="str">
+        <x:v>Category</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>Document Type</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>Description</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>In-Paper Industry Descriptor</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>Industry Code Or Description</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>Industry Code Type</x:v>
+      </x:c>
+      <x:c t="str">
         <x:v>Process Descriptions</x:v>
       </x:c>
       <x:c t="str">
@@ -98,6 +116,24 @@
         <x:v>1</x:v>
       </x:c>
       <x:c t="str">
+        <x:v>ESD</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>This OECD ESD is intended to provide information on the sources, use patterns, and potential release pathways of chemicals to be used in metalworking fluids. The document presents standard approaches for estimating the environmental releases of and occupational exposures to chemicals used in metalworking fluids. These approaches may be used to provide conservative, screening level estimates of environmental releases of and occupational exposures to chemicals used in these types of operations. Such estimates might result in release and exposure amounts that are likely to be higher, or at least higher than average, than amounts that might actually occur in real-world settings.</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>Metal Products and Machinery</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>The operations in this industry span over 200 different SIC codes (actual codes not specified).</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>n.a.</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c t="str">
         <x:v>7</x:v>
       </x:c>
       <x:c t="str">
@@ -157,6 +193,24 @@
         <x:v>1</x:v>
       </x:c>
       <x:c t="str">
+        <x:v>ESD</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>This OECD Emission Scenario Document (ESD) is intended to provide information on the sources, use patterns, and potential release pathways of chemicals used in the adhesive formulation industry. The document presents standard approaches for estimating the environmental releases of and occupational exposures to additives and components used in adhesive formulations. These approaches are intended to provide conservative, screening-level estimates resulting in release and exposure amounts that are likely to be higher, or at least higher than average, than amounts that might actually occur in the real world setting.</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>Adhesive Formulation</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>32552 (Adhesive Formulation), 322222 (Coated and Laminated Paper Manufacturing)</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>NAICS</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c t="str">
         <x:v>15</x:v>
       </x:c>
       <x:c t="str">
@@ -216,6 +270,24 @@
         <x:v>1</x:v>
       </x:c>
       <x:c t="str">
+        <x:v>ESD</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>This OECD Emission Scenario Document (ESD) is intended to provide information on the sources, use patterns and release pathways of chemicals used in the electronics industry, to assist in the estimation of releases of chemicals into the environment.</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>Toilet Preparations Manufacturing, and specifically under the Perfume Oil Mixtures and Blends Manufacturing subcategory</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>32562</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>NAICS</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c t="str">
         <x:v>13</x:v>
       </x:c>
       <x:c t="str">
@@ -275,6 +347,24 @@
         <x:v>1</x:v>
       </x:c>
       <x:c t="str">
+        <x:v>ESD</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>This Organisation for Economic Co-operation and Development (OECD) Emission Scenario Document (ESD) is intended to provide information on the sources, use patterns, and potential release pathways of chemicals used as chemical vapour deposition (CVD) precursors in the semiconductor industry. The document presents standard approaches for estimating environmental releases and occupational exposures, and discusses the typical engineering controls used to mitigate exposure to CVD precursors.</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>Semiconductor Manufacturing</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>334413</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>NAICS</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c t="str">
         <x:v>2</x:v>
       </x:c>
       <x:c t="str">
@@ -334,6 +424,24 @@
         <x:v>1</x:v>
       </x:c>
       <x:c t="str">
+        <x:v>ESD</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>This OECD Emission Scenario Document (ESD) is intended to provide information on the sources, use patterns, and potential release pathways of chemicals used in petroleum production at oil wells. The document presents standard approaches for estimating the environmental releases of and occupational exposures to oil production chemicals.</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>Crude Petroleum &amp; Natural Gas Extraction Industry</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>211111</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>NAICS</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c t="str">
         <x:v>3</x:v>
       </x:c>
       <x:c t="str">
@@ -393,6 +501,24 @@
         <x:v>1</x:v>
       </x:c>
       <x:c t="str">
+        <x:v>ESD</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>This OECD Emission Scenario Document (ESD) is intended to provide information on the sources, use patterns, and potential release pathways of chemicals to be used in water washing machines at industrial and institutional laundries. The document presents standard approaches for estimating the environmental releases of and occupational exposures to chemicals used in water washing machines in laundries. These approaches may be used to provide conservative, screening-level estimates of environmental releases of and occupational exposures to chemicals used in these types of operations. Such estimates might result in release and exposure amounts that are likely to be higher, or at least higher than average, than amounts that might actually occur in real-world settings.</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>Linen and Uniform Supply, Linen Supply, Industrial Launderers</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>81233, 812331, 812332</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>NAICS</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c t="str">
         <x:v>10</x:v>
       </x:c>
       <x:c t="str">
@@ -449,6 +575,24 @@
         <x:v>OECD (U.S. Author)</x:v>
       </x:c>
       <x:c t="str">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>ESD</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>This OECD Emission Scenario Document (ESD) is intended to provide information on the sources, use patterns, and potential release pathways of chemicals used in the automotive refinishing industry. The document presents standard approaches for estimating the environmental releases of and occupational exposures to the nonvolatile additives and components used in automotive refinishing paints and coatings. These approaches are intended to provide conservative, screening level estimates resulting in release and exposure amounts that are likely to be higher, or at least higher than average, than amounts that might actually occur in the real-world setting.</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>Automotive body, paint, and interior repair and maintenance</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>811121</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>NAICS</x:v>
+      </x:c>
+      <x:c t="str">
         <x:v>5</x:v>
       </x:c>
       <x:c t="str">
@@ -508,6 +652,24 @@
         <x:v>OECD (U.S. Author)</x:v>
       </x:c>
       <x:c t="str">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>ESD</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>This OECD Emission Scenario Document (ESD) is intended to provide information on the sources, use patterns, and potential release pathways of chemicals used in the manufacture of thermal and carbonless copy paper. The document presents approaches for estimating the environmental releases of and occupational exposures to additives and components used in thermal and carbonless copy paper coatings. These approaches are intended to provide conservative, screening-level estimates resulting in release and exposure amounts that are likely to be higher, or at least higher than average, than amounts that might actually occur in the real world setting.</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>Thermal paper and converter facilities</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
         <x:v>5</x:v>
       </x:c>
       <x:c t="str">
@@ -570,6 +732,24 @@
         <x:v>1</x:v>
       </x:c>
       <x:c t="str">
+        <x:v>ESD</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>This OECD Emission Scenario Document (ESD) is intended to provide information on the sources, use patterns, and potential release pathways of chemicals used in the semiconductor manufacturing industry. The document presents standard approaches for estimating environmental releases of and occupational exposures to additives and components used in photoresist formulations.</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>Semiconductor and Related Device Manufacturing</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>334413</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>NAICS</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c t="str">
         <x:v>6</x:v>
       </x:c>
       <x:c t="str">
@@ -626,6 +806,24 @@
         <x:v>OECD (U.S. Author)</x:v>
       </x:c>
       <x:c t="str">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>ESD</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>This OECD Emission Scenario Document (ESD) is intended to provide information on the sources, use patterns, and potential release pathways of chemicals used in the radiation curable products industry, specifically during application of radiation curable coatings, inks, and adhesives. The document focuses primarily on ultraviolet (UV) and electron beam (EB) curable products and presents standard approaches for estimating the environmental releases of and occupational exposures to components and additives used in radiation curable products.</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>Radiation Curable Products</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>322221, 322222, 322223, 322226, 337110, 337122, 337211, 321219, 326192, 3219185, 3219187, 336321, 3363601, 332431, 332439, 332812, 332996, 3332931, 335921, 3391153, 3391155, 334613, 334413, 334418b, 323110, 323113, 323112, 3231193, 3231199, 323119c, 323114, 323115, 313312, 3222226, 3222223, 3222225, 335921, 3391153, 3391155, 334613, 322221, 322223, 322225, 3261300</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>NAICS</x:v>
+      </x:c>
+      <x:c t="str">
         <x:v>6</x:v>
       </x:c>
       <x:c t="str">
@@ -688,6 +886,24 @@
         <x:v>1</x:v>
       </x:c>
       <x:c t="str">
+        <x:v>ESD</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>This OECD Emission Scenario Document (ESD) is intended to provide information on the sources, use patterns, and potential release pathways of chemicals used in adhesive products, specifically during the use of adhesives in various industries. It is also intended to serve as a preliminary screening tool for assessing such chemicals. The document focuses primarily on water-based and organic solvent-based solution, hot-melt, pressure-sensitive, and reactive (excluding radiation curable1) adhesives during industrial applications for the purposes of joining substrates. The adhesives may be applied using spray, roll, curtain, or syringe or bead application methods. The document presents standard approaches for estimating the environmental releases of and occupational exposures to additives and components used in adhesive formulations. These approaches are intended to provide conservative, screening-level estimates resulting in release and exposure amounts that are likely to be higher, or at least higher than average, than amounts that might actually occur in the real world setting.</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>Computer/Electronic and Electrical Product Manufacturing; Motor and Non-Motor Vehicle, Vehicle Parts, and Tire Manufacturing (Except Retreading); Labels and Tapes Manufacturing</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>334111, 334112, 334113, 334119, 334210, 334220, 334290, 334310, 334411, 334412, 334413, 334415, 334416, 334417, 334418, 334419, 334510, 334511, 334512, 334513, 334514, 334515, 334516, 334517, 334518, 334519, 334611, 334612, 334613, 335110, 335121, 335122, 335129, 335211, 335212, 335221, 335222, 335224, 335228, 335311, 335312, 335313, 335314, 335911, 335912, 335921, 335929, 335931, 335932, 335991, 335999, 336111, 336112, 336120, 336211, 336212, 336213, 336214, 336311, 336312, 336321, 336322, 336330 336340, 336350, 336360, 336370, 336391, 336399, 326211, 322222</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>NAICS</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c t="str">
         <x:v>13</x:v>
       </x:c>
       <x:c t="str">
@@ -747,6 +963,24 @@
         <x:v>1</x:v>
       </x:c>
       <x:c t="str">
+        <x:v>ESD</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>This OECD Emission Scenario Document (ESD) is intended to provide information on the sources, use patterns, and potential release pathways of non-volatile chemicals used in textile dyes. The document focuses primarily on the application of dyes to fibers, yarns and fabrics by batch or continuous processes. The document presents standard approaches for estimating the environmental releases of and occupational exposures to non-volatile chemicals used in dye formulations.</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>Broadwoven Fabric Finishing Mills; Textile and Fabric Finishing (except Broadwoven Fabric Mills)</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>313311; 313312</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>NAICS</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c t="str">
         <x:v>7</x:v>
       </x:c>
       <x:c t="str">
@@ -803,6 +1037,24 @@
         <x:v>OECD (U.S. Author)</x:v>
       </x:c>
       <x:c t="str">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>ESD</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>This OECD draft Emission Scenario Document (ESD) is intended to provide information on the sources, use patterns, and potential release pathways of chemicals used as vapor degreasers. The document presents standard approaches for estimating environmental releases and occupational exposures. EPA developed this ESD using relevant data and available information on the solvent degreasing industry, including process descriptions, operating information, chemicals usage, wastes generation, worker activities, and exposure information. EPA supplemented the data collected with standard models to develop the environmental release and occupational exposure estimates presented in this ESD.</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>Vapor Degreaser</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>314999, 321113, 323111, 325180, 325998, 326299, 331110, 331210, 331410, 331420, 332111, 332112, 332119, 332117, 332215, 332216, 332311, 332313, 332431, 332510, 332618, 332721, 332722, 332811, 332812, 332813, 332912, 332913, 332919, 332994, 332996, 332999, 333132, 333249, 333318, 333415, 333921, 333994, 333999, 334220, 334413, 334416, 334417, 334419, 334513, 334515, 335120, 225121, 335210, 335312, 335313, 335911, 335921, 335929, 335999, 336320, 336340, 336411, 336413, 336414, 336510, 337125, 337127, 339114, 339990, 339992, 339995, 339999, 488111, 493110, 811310</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>NAICS</x:v>
+      </x:c>
+      <x:c t="str">
         <x:v>1</x:v>
       </x:c>
       <x:c t="str">
@@ -862,6 +1114,24 @@
         <x:v>OECD (U.S. Author)</x:v>
       </x:c>
       <x:c t="str">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>ESD</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>This OECD draft Emission Scenario Document (ESD) is intended to provide information on the sources, use patterns, and potential release and exposure pathways of non-volatile chemicals used in aqueous film-forming foams (AFFFs) in firefighting applications. The document presents standard approaches for estimating the environmental releases of and occupational exposures to chemicals used in AFFF. This document may be used to provide conservative, screening-level estimates of environmental releases of and occupational exposures to chemical components contained in AFFF formulations. Such estimates might result in release and exposure amounts that are likely to be higher, or at least higher than average, than amounts that might actually occur in real world practice.</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>Commerical/Industrial Uses of AFFF Concentrate in Firefighting (Military, Civil Aviation, Municipal Fire Departments, Petroleum Refineries, Petrochemical Manufacturing)</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>Not specified</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>n.a.</x:v>
+      </x:c>
+      <x:c t="str">
         <x:v>1</x:v>
       </x:c>
       <x:c t="str">
@@ -924,6 +1194,24 @@
         <x:v>2</x:v>
       </x:c>
       <x:c t="str">
+        <x:v>ESD</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>This OECD Emission Scenario Document (ESD) is intended to provide information on the sources, use patterns, and potential release pathways of additive chemicals used in automotive finished lubricants. The document presents standard approaches for estimating the environmental releases of and occupational exposures to chemical additives used in automotive finished lubricants.</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>Petroleum lubricating oil and grease manufacturing; General automotive repar; Automotive transmission repari; Automotive oil change and lubrication shops</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>324191; 811111; 811113; 811191</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>NAICS</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c t="str">
         <x:v>15</x:v>
       </x:c>
       <x:c t="str">
@@ -980,6 +1268,24 @@
         <x:v>EPA</x:v>
       </x:c>
       <x:c t="str">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>GS</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>Paint is comprised of binders, pigments, solvents, and various additives. Most automobile paint components for which PMNs have been submitted in the past are nonvolatile; a volatile PMN used for automobile paint may in fact be a monomer which would be consumed during the paint formulation step. Therefore, this generic scenario is most applicable in evaluating nonvolatile PMNNs that are part of the paint solids; caution should be used when using this generic scenario in evaluation of other paint components. During automobile refinishing and in many (but not all) automobile manufacturing operations, the paint is sprayed onto the automobile. This generic scenario is applicable only for spray painting operations. This generic scenario will not address the manufacture of the paint components or the formulation of the components into paint.</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>Automobile OEM Painting</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>Not specified</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>n.a.</x:v>
+      </x:c>
+      <x:c t="str">
         <x:v>1</x:v>
       </x:c>
       <x:c t="str">
@@ -1039,6 +1345,27 @@
         <x:v>EPA</x:v>
       </x:c>
       <x:c t="str">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>GS</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>The semiconductor industry is one of the fastest growing industries in the world. Manufacturing of integrated circuits (ICs) constitutes a major segment of the semiconductor industry. The U.S. IC manufacturers comprise a $15.8 billion industry that represents approximately a 100% increase
+from the year 1982. The size of the industry is based on factory shipments of ICs from the manufacturers in the United States. In the IC industry, the cleaning process is one of the most critical and important steps in IC
+fabrication. Uncleaned wafers and parts create defective devices and drastically lower the production yield. Wafer contamination originates from the particulates (dirt, grease, soil, aerosols, etc.) generated by the equipment in the work area and/or the residues from the process chemicals
+(resist, fluxes, metal oxides, etc.) that are used in the earlier steps. This Generic Scenario covers environmental releases and occupational exposures to chemicals used in wet cleaning processese in IC fabrication.</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>Semiconductor and Related Device Manufacturing</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>Not specified</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>n.a.</x:v>
+      </x:c>
+      <x:c t="str">
         <x:v>1</x:v>
       </x:c>
       <x:c t="str">
@@ -1098,6 +1425,24 @@
         <x:v>EPA</x:v>
       </x:c>
       <x:c t="str">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>GS</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>Approximately 325 billion gallons of water are used daily in the United States. Depending on its use, most water must be treated, including water used by industry, municipalities, and power-generating utilities.</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>Non-Specific Industry, Municipalities, and Power-Generating Utilities</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>Not specified</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>n.a.</x:v>
+      </x:c>
+      <x:c t="str">
         <x:v>1</x:v>
       </x:c>
       <x:c t="str">
@@ -1157,6 +1502,24 @@
         <x:v>EPA</x:v>
       </x:c>
       <x:c t="str">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>GS</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>Approximately 325 billion gallons of water are used daily in the United States. Depending on its use, most water must be treated, including water used by industry, municipalities, and power-generating utilities.</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>Non-Specific Industry, Municipalities, and Power-Generating Utilities</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>Not specified</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>n.a.</x:v>
+      </x:c>
+      <x:c t="str">
         <x:v>1</x:v>
       </x:c>
       <x:c t="str">
@@ -1216,6 +1579,24 @@
         <x:v>EPA</x:v>
       </x:c>
       <x:c t="str">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>GS</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>This Generic Scenario (GS) is intended to provide information on the sources, use patterns, and potential environmental release and occupational exposure pathways of additives used in the conversion of compounded plastic resins into finished products.</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>Plastics Converting Industry</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>326111; 326112; 326113; 326121; 326122; 326130; 326160; 326191; 326192; 326199</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>NAICS</x:v>
+      </x:c>
+      <x:c t="str">
         <x:v>1</x:v>
       </x:c>
       <x:c t="str">
@@ -1275,6 +1656,24 @@
         <x:v>EPA</x:v>
       </x:c>
       <x:c t="str">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>GS</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>The petroleum industry has adopted the use of enhanced oil recovery as a way of extending the life of current oil reserves. Enhanced oil recovery research began in the 1920’s during the first petroleum shortage in the United States. The first methods that were developed employed waterflooding; however, even at that time chemicals often were used in conjunction with water. Today, polymer/surfactant flooding is one of the most efficient and expensive methods of enhanced oil recovery. However, steam stimulation and flooding also show promise are more economical than polymer/surfactant flooding. In 1991 alone, 93 new chemicals were being marketed for enhanced oil recovery processes (Petroleum Engineer International, 1991).</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>Oil/Gas Production</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>Not specified</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>n.a.</x:v>
+      </x:c>
+      <x:c t="str">
         <x:v>1</x:v>
       </x:c>
       <x:c t="str">
@@ -1334,6 +1733,24 @@
         <x:v>EPA</x:v>
       </x:c>
       <x:c t="str">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>GS</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>Each year, approximately 300 companies in the United States drill and complete several thousand wells for oil or gas production (Calvert and Smith, 1990). Many different types of chemicals may be used during well casing and cementing processes to improve the strength and cohesiveness of the cement. Chemicals may be used as a component of the spacer fluid or chemical wash, or may bes used as an additive to the cement. Cement additives are classified by the following categories: accelerators; light weight; heavy weight; retarders; lost circulation; filtration control additives; friction reducers; and specialy materials.</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>Oil/Gas Production</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>Not specified</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>n.a.</x:v>
+      </x:c>
+      <x:c t="str">
         <x:v>1</x:v>
       </x:c>
       <x:c t="str">
@@ -1393,6 +1810,24 @@
         <x:v>EPA</x:v>
       </x:c>
       <x:c t="str">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>GS</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>Metal cleaning is performed to remove contaminants such as dust, oils, waxes, metal fines, and other particulates from workpiece surfaces. Cleaning is performed in numerous industries for a variety of purposes. For example, in finishing processes such as metal plating and painting, a clean surface is desired to improve coating adherence. In maintenance activities, cleaning is performed to improved the effectiveness of the test procedure or repair operation. The exact purpse of a cleaning step and the degree of cleanliness require usually determine how an industry selects a cleaning process</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>Metal Cleaning/Degreasing</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>Not specified</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>n.a.</x:v>
+      </x:c>
+      <x:c t="str">
         <x:v>1</x:v>
       </x:c>
       <x:c t="str">
@@ -1452,6 +1887,24 @@
         <x:v>EPA</x:v>
       </x:c>
       <x:c t="str">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>GS</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>Spray polyurethane foam (SPF) insulation is commonly used in renovation or new building construction and is made by mixing fast-reacting chemicals that expand on contact to create a continuous stream of foam. This foam is applied to walls, ceilings, roofs and other building structures to provide highly effective insulation from heat, air, and/or moisture.</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>Residential Building Construction; Nonresidential (Commercial) Building Construction</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>236100; 236200</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>NAICS</x:v>
+      </x:c>
+      <x:c t="str">
         <x:v>1</x:v>
       </x:c>
       <x:c t="str">
@@ -1511,6 +1964,24 @@
         <x:v>EPA</x:v>
       </x:c>
       <x:c t="str">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>GS</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>Almost 600 million cubic feet of wood are treated with preservatives in the United States each year. Almost 75% of the wood (400 million cubic feet) is treated with waterborne preservatives, which are used to treat poles, piling, fence posts, lumber, timber, and plywood. Less than 25% of the wood is created with oilborne preservatives such as pentachlorophenol (PCP) and creosote. The most common waterborne preservatives are are chomated copper arsenate (CCA), ammoniacal copper arsenate (ACA), and ammoniacal copper-zinc-arsenate (ACZA), which are derived from ammonium arsenic pentoxide, sodium arsenate, or sodium pyroarsenate and other metal salts (e.g., chromium, copper, and zinc). Arsenictrioxide is converted to arsenic acid to produce these arsenical wood preservatives. All arsenic trioxide consumed in the United States is imported, and the wood-preserving industry uses 70% of this import. The current U.S. demand for CCA is 150 million pounds (of active ingredient as oxide content). The U.S. production is about 165 million pounds. CCA is provided by manufacturers as a 50 or 60% concentration.</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>Wood-Preserving</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>Not specified</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>n.a.</x:v>
+      </x:c>
+      <x:c t="str">
         <x:v>0</x:v>
       </x:c>
       <x:c t="str">
@@ -1570,6 +2041,24 @@
         <x:v>EPA</x:v>
       </x:c>
       <x:c t="str">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>GS</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>This Generic Scenario (GS) is intended to provide information on the sources, use patterns, and potential release pathways of chemical additives used in compounded thermoplastic resins. It also is intended to serve as a preliminary screening tool for assessing such chemicals. The reader should note that this document does not cover the subsequent conversion of compounded plastic resins into finished articles, which is covered separately in a GS on the Use of Additives in Plastics Converting.</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>Custom Compounding of Purchased Resins</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>325991</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>NAICS</x:v>
+      </x:c>
+      <x:c t="str">
         <x:v>1</x:v>
       </x:c>
       <x:c t="str">
@@ -1629,6 +2118,24 @@
         <x:v>EPA</x:v>
       </x:c>
       <x:c t="str">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>GS</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>This document presents methods for estimating occupational exposures to chemical additives in brake pads during lightweight automotive (e.g., cars) brake pad replacement. This draft GS may be periodically updated to reflect changes in the industry and new information available. Users of the document are encouraged to submit comments, corrections, updates, and new information to RAD.</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>Automotive repair and maintenance</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>8111</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>NAICS</x:v>
+      </x:c>
+      <x:c t="str">
         <x:v>1</x:v>
       </x:c>
       <x:c t="str">
@@ -1688,6 +2195,26 @@
         <x:v>EPA</x:v>
       </x:c>
       <x:c t="str">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>GS</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>The purpose of this report is to develop a standardized approach that EPA's Chemical Engineering Branch (CEB) can use to estimate potential occupational exposures and environmental releases during closed-loop fermentation processes that involve the use of genetically engineered microorganisms (GEMs). These estimation techniques may be used by CEB to evaluate future biotechnology premanufacture notices (PMNs). The document also discusses in detail a typical fermentation process, and the control technologies, inactivation procedures and sterilization procedures, that can be expected.
+Information and data used to develop the estimation procedures were obtained from a literature search of fermentation processes using recombinant microorganisms, including a review of the 16 biotechnology PMNs that were submitted to EPA between 1987 and 1995.
+Based on information and data acquired from the literature search, reasonable worst-case release and exposure estimations can be made using the methodology and calculations that are discussed in detail in Sections 3.0 and 4.0. These calculations are summarized in the following table.</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>Biotechnology</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>n.a.</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>n.a.</x:v>
+      </x:c>
+      <x:c t="str">
         <x:v>1</x:v>
       </x:c>
       <x:c t="str">
@@ -1747,6 +2274,25 @@
         <x:v>EPA</x:v>
       </x:c>
       <x:c t="str">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>GS</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>The U.S. Environmental Protection Agency (EPA) with support from Eastern Research Group, Inc. (ERG) has developed this draft Quick-Strike Generic Scenario for estimating environmental releases of chemical additives used in mineral and metal ore flotation processes, as well as the occupational inhalation exposure to these chemical additives during the flotation process. This scenario is a quick-strike generic scenario as opposed to a regular generic scenario, meaning its scope is designed to serve the needs of EPA programs on a real-time basis. A quick-strike generic scenario differs from a regular generic scenario in that that it has a limited scope that serves the needs of an ongoing evaluation and can be completed in a shorter timeframe than a regular generic scenario.
+The Risk Assessment Division (RAD) of EPA’s Office of Pollution Prevention and Toxics (OPPT) is responsible for preparing occupational exposure and environmental release assessments of chemicals for a variety of EPA’s Toxic Substances Control Act (TSCA) Chemical Review Programs, including Premanufacture Notice (PMN) reviews. This document presents methods for estimating environmental releases of chemical additives during their use in mineral and metal ore flotation processes, as well as the occupational inhalation exposure to these chemical additives during the flotation process.</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>Nonmetallic mineral mining and quarrying; Metal ore mining</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>2123; 2122</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>NAICS</x:v>
+      </x:c>
+      <x:c t="str">
         <x:v>1</x:v>
       </x:c>
       <x:c t="str">
@@ -1806,6 +2352,24 @@
         <x:v/>
       </x:c>
       <x:c t="str">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>GS</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v>Automobile Industry, Agriculture, Commerical Equipment, Office and Home Appliances</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>n.a.</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>n.a.</x:v>
+      </x:c>
+      <x:c t="str">
         <x:v>1</x:v>
       </x:c>
       <x:c t="str">
@@ -1865,6 +2429,29 @@
         <x:v/>
       </x:c>
       <x:c t="str">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>GS</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>Electroplating is a diverse industry. Many plating specialty chemical suppliers and many plating shops
+produce and use a variety of plating solutions. Currently, there are no data available on the size of the
+market and the market growth rates. This information is being compiled by the Metal Finishing Suppliers
+Association and will be available in 1994. The major metals plated include nickel, chromium, zinc, and
+copper. Many other metals are plated, including cadmium, gold, silver, indium, iron, lead, tin, and
+rhodium.</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>Metal Finishing Suppliers Association</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>n.a.</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>n.a.</x:v>
+      </x:c>
+      <x:c t="str">
         <x:v>1</x:v>
       </x:c>
       <x:c t="str">
@@ -1924,6 +2511,24 @@
         <x:v>EPA</x:v>
       </x:c>
       <x:c t="str">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>GS</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>This model estimates a loss fraction of dust that may be generated during the transferring/unloading of solid powders. This model can be used to estimate a loss fraction of dust both when the facility does not employ capture technology (i.e. local exhaust ventilation, hoods) or dust control/removal technology (i.e., cyclones, electrostatic precipitators, scrubbers, or filters), and when the facility does employ capture and/or control/removal technology. Solid powders, for purposes of this model, are dry solids comprised of numerous loose particles with varying aerodynamic diameters that would become airborne during transfer operations. This model is not applicable to other solid forms, such as pellets, sheets, or wet slurries that are not expected to be airborne during transfer operations.</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>n.a.</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>n.a.</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>n.a.</x:v>
+      </x:c>
+      <x:c t="str">
         <x:v>0</x:v>
       </x:c>
       <x:c t="str">
@@ -1983,6 +2588,24 @@
         <x:v>EPA</x:v>
       </x:c>
       <x:c t="str">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>GS</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>Typical finishing agents including permanent press, flame retardants, and water/stain repellents. Consumption in 1989 of finishing agents used for the processing of textile mill products is estimated to be 154 million pounds valued at $208 million. In the next five years, an average growth of 2.7% is projected for chemicals and polymers used in finishing textile products. Demand for organic specialty chemicals, which includes flame retardants, surfactants, and permanent press resins is expected to grow at an average rate of about 3.3% annually. Expected demand for polymeric products, which includes softeners and water/stain repellents, is diminshed by reduced fabric application levels of these products as users develop improved formulation technology. (Frost and Sullivan, 1989)</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>Fabric Finishing</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>n.a.</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>n.a.</x:v>
+      </x:c>
+      <x:c t="str">
         <x:v>1</x:v>
       </x:c>
       <x:c t="str">
@@ -2042,6 +2665,25 @@
         <x:v>EPA</x:v>
       </x:c>
       <x:c t="str">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>GS</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>This scenario examines the film deposition process generically to evaluate various IC products for human exposure to hazardous chemicals and chemical waste generated. 
+This report looks at a realistic scenario with both automated and manual process controls. However, most IC fabrication processes are automated and are performed in clean rooms, and the IC manufacturing industry is considered one of the safest industries in the United States. In fact, according to Semiconductor International Magazine [5], there has never been a fatal injury in a U.S. IC fabrication facility. This statistic is impressive considering the number of hazardous chemicals commonly used in the manufacture of ICs. However, questions on long-term effects still remain unanswered. The worst-case scenario of personnel exposure to hazardous gases or chemicals potentially will arise from equipment maintenance and accidents [6]. The chemicals used, the potential human exposure, and the waste generated during film deposition in the IC fabrication process are described below.</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>Integrated Circuit Fabrication</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>n.a.</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>n.a.</x:v>
+      </x:c>
+      <x:c t="str">
         <x:v>2</x:v>
       </x:c>
       <x:c t="str">
@@ -2101,6 +2743,24 @@
         <x:v>EPA</x:v>
       </x:c>
       <x:c t="str">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>GS</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>The purpose of this scenario is to standardize the approach used to assess potential dose rates for workers handling solid and dried powders during filtration and drying operations. Development of a general comprehensive model for particulate exposures is an ongoing CEB research effort, therefore, this scenario is intended to be an interim, generic approach for using the information collected by ORD. This information is most likely useful for relatively small volume chemicals handled in batch sizes on the order of 100 kg/batch.</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>n.a.</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>n.a.</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>n.a.</x:v>
+      </x:c>
+      <x:c t="str">
         <x:v>1</x:v>
       </x:c>
       <x:c t="str">
@@ -2160,6 +2820,24 @@
         <x:v>EPA</x:v>
       </x:c>
       <x:c t="str">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>GS</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>This generic scenario is based on research that was conducted by Eastern Research Group (ERG) in the spring and summer of 1998. The purpose of the study was to develop a Cleaner Technologies Substitute Assessment (CTSA) for U.S. EPA’s Design for the Environment (DfE) initiative. Research for the CTSA included contacting industry representatives to acquire realistic process descriptions, occupational exposure patterns, and printing ink formulations (many of which contained TSCA Confidential Business Information). The CTSA determined that there are three primary ink formulations, each having slightly different characteristics: solvent-based, UV-cured, and water-based. Additionally, ink consumption rates vary depending on the color. The colors analyzed were: white, green, blue, magenta, and cyan. The scope of the CTSA was to estimate occupational exposure, both inhalation and dermal, and fugitive and stack air releases from volatile chemicals used in flexographic printing operations. While the CTSA recognized that there could be releases of volatile chemicals to land or water from these operations, they are unlikely except in the event of equipment cleaning and container residue. The CTSA assumed that 100% of the volatile chemicals will evaporate during the process or remain on the substrate. Therefore, liquid and solid releases are not specifically addressed. The methodology used in the Chemical Engineering Branch (CEB) Engineering Manual for estimation of exposures and releases from open surfaces was used as a basis for modeling. Several discussions and meetings were held with industry, ERG, and EPA personnel to develop the default values needed to conduct the modeling during a “typical” flexographic printing operation. Specific details and assumptions are discussed in the CTSA.</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>Flexographic Printing</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>n.a.</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>n.a.</x:v>
+      </x:c>
+      <x:c t="str">
         <x:v>1</x:v>
       </x:c>
       <x:c t="str">
@@ -2219,6 +2897,24 @@
         <x:v>EPA</x:v>
       </x:c>
       <x:c t="str">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>GS</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>The development of a scenario for the photoresist formulation industry will supplement the existing scenario, “Photoresist Use in the Semiconductor Industry”. Photoresists are used in the manufacturing of printed circuit board, optical photographic films, X-ray films and various electronic components. Much of the new chemistry development activities are, however, are for application in the semiconductor industry.</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>Camera Film, Printed Circuit Boards, Electronic Components, and Semiconductors</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>n.a.</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>n.a.</x:v>
+      </x:c>
+      <x:c t="str">
         <x:v>1</x:v>
       </x:c>
       <x:c t="str">
@@ -2278,6 +2974,24 @@
         <x:v>EPA</x:v>
       </x:c>
       <x:c t="str">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>GS</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>This Generic Scenario is intended to provide information on the sources, use patterns, and potential release pathways of chemicals used in the formulation of waterborne coatings. The document presents approaches for estimating the environmental releases of and occupational exposures to components and additives used in waterborne coatings. These approaches are intended to provide conservative, screening-level estimates resulting in release and exposure amounts that are likely to be higher, or at least higher than average, than amounts that might actually occur in the real world setting</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>Paint and Coating Manufacturers</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>325510</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>NAICS</x:v>
+      </x:c>
+      <x:c t="str">
         <x:v>0</x:v>
       </x:c>
       <x:c t="str">
@@ -2337,6 +3051,25 @@
         <x:v>EPA</x:v>
       </x:c>
       <x:c t="str">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>GS</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>The purpose of this effort is to revise the current default loss fractions used by the EPA/OPPT Drum Residual Model. The general assessment hierarchy practiced by EPA to develop assessment models works towards basing these models off of actual data rather than the assumption of compliance with established regulatory limits. The current model for drum residuals bases the “high-end” estimated loss fraction on current RCRA regulations for empty containers. Ideally, “high-end” estimates, as well as other standard estimates, should be based on data provided by industry, collected through established EPA programs (e.g. Pre-Manufacture
+Notices under the new chemicals program), or generated through empirical experimentation.</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>n.a.</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>n.a.</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>n.a.</x:v>
+      </x:c>
+      <x:c t="str">
         <x:v>0</x:v>
       </x:c>
       <x:c t="str">
@@ -2396,6 +3129,26 @@
         <x:v>EPA</x:v>
       </x:c>
       <x:c t="str">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>GS</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>This scenario presents methods that can be used to estimate releases and exposures to the following papermaking additives: acids and bases, alum, sizing agents, dry-strength adhesives, wet-strength resins, fillers, coloring materials, retention aids, flocculants, defoamers, drainage aids,
+optical brighteners, pitch control chemicals, slimicides, and specialty chemicals. The generic scenario is applicable to chemicals that are used during the stock preparation step or as on machine additives in the papermaking process. The scenario covers the introduction of the
+additive to the papermaking process through to the final disposition of the additive either in the paper product or as waste.</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>Paper and paperboard manufacturing industry</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>32212; 32213</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>NAICS</x:v>
+      </x:c>
+      <x:c t="str">
         <x:v>0</x:v>
       </x:c>
       <x:c t="str">
@@ -2455,6 +3208,24 @@
         <x:v>EPA</x:v>
       </x:c>
       <x:c t="str">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>GS</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>The generic scenario will provide a methodology for calculating the environmental releases and worker exposures to chemicals incorporated into the foamed plastic during its manufacture. These chemicals include prepolymers and other reactive materials, plastic performance additives, and certain processing aids (e.g., catalysts, blowing agents).</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>Polystyrene Foam Product Manufacturing; and Urethane and Other Foam Product (except polystyrene) Manufacturing</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>326140; 326150</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>NAICS</x:v>
+      </x:c>
+      <x:c t="str">
         <x:v>0</x:v>
       </x:c>
       <x:c t="str">
@@ -2514,6 +3285,24 @@
         <x:v>EPA</x:v>
       </x:c>
       <x:c t="str">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>GS</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v>Granular Detergent Manufacturing</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>n.a.</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>n.a.</x:v>
+      </x:c>
+      <x:c t="str">
         <x:v>1</x:v>
       </x:c>
       <x:c t="str">
@@ -2573,6 +3362,24 @@
         <x:v>EPA</x:v>
       </x:c>
       <x:c t="str">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>GS</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>The following sections of this document describe the flexible polyurethane foam industry, the manufacturing process of flexible polyurethane foam, the releases and associated occupational exposures from the manufacturing process, related control technologies and personal protective equipment, and regulations governing the use and potential release of diisocyanates in the industry.</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>Plastics Foam Products/Urethane Foam Product Manufacturing</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>3086/326150</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>SIC/NAICS</x:v>
+      </x:c>
+      <x:c t="str">
         <x:v>2</x:v>
       </x:c>
       <x:c t="str">
@@ -2632,6 +3439,24 @@
         <x:v>EPA</x:v>
       </x:c>
       <x:c t="str">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>GS</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>The following sections of this document describe the rigid polyurethane foam industry, the manufacturing processes of rigid polyurethane foam, the releases and associated occupational exposures from the manufacturing processes, related control technologies and personal protective equipment, and regulations governing the use and potential release of diisocyanates in the industry.</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>Urethane and Other Foam Product (except polystyrene) Manufacturing</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>3086/326150</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>SIC/NAICS</x:v>
+      </x:c>
+      <x:c t="str">
         <x:v>4</x:v>
       </x:c>
       <x:c t="str">
@@ -2691,6 +3516,24 @@
         <x:v>EPA</x:v>
       </x:c>
       <x:c t="str">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>GS</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>The purpose of this report is to develop a standardized approach that EPA’s Chemical Engineering Branch (CEB) can use to estimate potential occupational exposures and environmental releases from the use of leather dyeing chemicals. These estimation techniques may be used by CEB to future evaluate leather dyeing premanufacture notices (PMNs) and existing leather dyeing PMNs. The document also presents an industry profile, a discussion of typical processes in the industry, including release and exposure points, control technologies, and source reduction, pollution prevention, and material substitution alternatives (when applicable).</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>Leather and Hide Tanning and Finishing</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>31610</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>NAICS</x:v>
+      </x:c>
+      <x:c t="str">
         <x:v>1</x:v>
       </x:c>
       <x:c t="str">
@@ -2753,6 +3596,24 @@
         <x:v>3</x:v>
       </x:c>
       <x:c t="str">
+        <x:v>GS</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>The purpose of this report is to develop a standardized approach that EPA’s Chemical Engineering Branch (CEB) can use to estimate potential occupational exposures and environmental releases from the use of leather tanning chemicals. These estimation techniques may be used by CEB to evaluate future leather tanning premanufacture notices (PMNs) and existing leather tanning PMNs. The document also presents an industry profile, a discussion of typical processes in the industry, including release and exposure points, control technologies, and worker personal protective equipment that is typically used (when applicable); and source reduction, pollution prevention, and material substitution alternatives (when applicable). Note that chemicals involved with leather dyeing are addressed in CEB’s Generic Scenario for Leather Dyeing.</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>Leather and Hide Tanning and Finishing</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>31610</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>NAICS</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c t="str">
         <x:v>2</x:v>
       </x:c>
       <x:c t="str">
@@ -2809,6 +3670,24 @@
         <x:v>EPA</x:v>
       </x:c>
       <x:c t="str">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>GS</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>This document provides updates to the environmental release estimates presented in the 2010 Organisation for Economic Co-operation and Development (OECD) Emission Scenario Document (ESD) on the Photoresist Use in Semiconductor Manufacturing. These revisions to the environmental release estimates presented in the 2010 ESD on Photoresist Use in Semiconductor Manufacturing are based on information provided by the Semiconductor Onium Photoacid Generator (PAG) Consortium.</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>Semiconductor and Related Device Manufacturing</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>334413</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>NAICS</x:v>
+      </x:c>
+      <x:c t="str">
         <x:v>0</x:v>
       </x:c>
       <x:c t="str">
@@ -2868,6 +3747,24 @@
         <x:v>EPA</x:v>
       </x:c>
       <x:c t="str">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>GS</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>This document presents a profile of the transportation equipment cleaning industry along with descriptions of widely-used processes.</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>Transportation Equipment Cleaning Industry</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>n.a.</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>n.a.</x:v>
+      </x:c>
+      <x:c t="str">
         <x:v>1</x:v>
       </x:c>
       <x:c t="str">
@@ -2927,6 +3824,24 @@
         <x:v>EPA</x:v>
       </x:c>
       <x:c t="str">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>GS</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>This document presents estimation methods for environmental releases and occupational exposures to chemcials used in transformer manufacturing.</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>The North American Electrical and Electronic Transformer and Coil Industry</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>n.a.</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>n.a.</x:v>
+      </x:c>
+      <x:c t="str">
         <x:v>1</x:v>
       </x:c>
       <x:c t="str">
@@ -2986,6 +3901,26 @@
         <x:v>EPA</x:v>
       </x:c>
       <x:c t="str">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>GS</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>The purpose of this report is to develop a standardized approach that EPA’s chemical engineering branch (CEB) can use to estimate potential occupational exposures and environmental releases from the manufacture, processing, and use of paper dyes. These estimation techniques may be used by CEB to evaluate future paper dye premanufacture notices (PMNs) and existing paper dyes. The document also presents an industry profile, a discussion of typical processes in the industry, including release and exposure points, control technologies, and
+worker personal protective equipment that is typically used (when applicable); and source
+reduction, pollution prevention, and material substitution alternatives (when applicable).</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>Manufacture and Use of Paper Dyes</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>n.a.</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>n.a.</x:v>
+      </x:c>
+      <x:c t="str">
         <x:v>2</x:v>
       </x:c>
       <x:c t="str">
@@ -3045,6 +3980,24 @@
         <x:v>EPA</x:v>
       </x:c>
       <x:c t="str">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>GS</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>The proposed ESD would track the use of chemicals used to formulate printing inks and the subsequent use of these inks in printing operations, and update releases and exposures to these chemicals. The following diagram demonstrates the applicability of this scenario.</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>Printing Ink Manufacturing; Commercial Lithographic Printing; Commercial Gravure Printing; Commercial Flexographic Printing; Commercial Screen Printing; Quick Printing; Digital Printing; Other Commercial Printing</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>325910; 323110; 323111; 323112; 323113; 323114; 323115; 323119</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>NAICS</x:v>
+      </x:c>
+      <x:c t="str">
         <x:v>7</x:v>
       </x:c>
       <x:c t="str">
@@ -3104,6 +4057,24 @@
         <x:v>EPA</x:v>
       </x:c>
       <x:c t="str">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>GS</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>There are three general manufacturing stages in creating a final printed circuit board assemply: (1) the fabrication of the basic materials used in the printed circuit board; (2) the fabrication of the basic printed circuit board; and (3) the fabrication of the printed circuit board assembly, which is used in almost all electronic equipment manufactured today. Each of these three stages is a separate industry that usually is independent of the other two. Due to the broad scope of these three stages and the chemical processes involved (especially printed circuit board fabrication), this presentation covers only the first stage - the material fabrication processes.</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>Printed Circuit Board Manufacturing</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>n.a.</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>n.a.</x:v>
+      </x:c>
+      <x:c t="str">
         <x:v>1</x:v>
       </x:c>
       <x:c t="str">
@@ -3163,6 +4134,24 @@
         <x:v>EPA</x:v>
       </x:c>
       <x:c t="str">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>GS</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>Newspapers are found globally and are printed in every major city as well as in many smaller cities in the United States. In 1992, there were 1,570 daily, 893 Sunday, and 7,406 weekly newspapers in operation in the United States. They represent a circulation of 60,083,265 daily, 62,542,031 Sunday, and 55,445,601 weekly newspapers. The newspaper industry employed 453,000 workers in 1992.</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>Newspaper Printing</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>n.a.</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>n.a.</x:v>
+      </x:c>
+      <x:c t="str">
         <x:v>2</x:v>
       </x:c>
       <x:c t="str">
@@ -3222,6 +4211,25 @@
         <x:v>EPA</x:v>
       </x:c>
       <x:c t="str">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>GS</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>FCC is used to convert crude oil (generally atmospheric and/or vacuum distilled) into lighter products such as gasoline and diesel fuel. They are increasingly being used for olefin production to feed octane additive production (MTBE, ETBE, TAME) as well as recovery of sulfur present in crude. FCC units (FCCU) can vary in throughput from a few thousand barrels of oil per day (BPD) to over 100,000 BPD. There are 42 gallons/barrel.
+Crude separation processes are the most basic part of petroleum refining and consist of distillation either at ambient pressure or under vacuum. Refineries vary in size from 20,000 BPD to over 400,000 BPD.</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>Fluid Catalytic Cracking and Crude Separation Processes</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>n.a.</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>n.a.</x:v>
+      </x:c>
+      <x:c t="str">
         <x:v>2</x:v>
       </x:c>
       <x:c t="str">
@@ -3281,6 +4289,24 @@
         <x:v>EPA</x:v>
       </x:c>
       <x:c t="str">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>GS</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>ERG collected readily available information that could be used to develop a generic scenario to describe the photographic industry, including information on environmental releases and potential worker exposures. This memorandum presents a summary of current trends in the photographic industry along with descriptions of widely-used processes involved in photographic film and papermaking, photographic film/paper coating, and development of paper and films. Based on information obtained during this preliminary search, this scoping document recommends an approach for the development of a generic scenario for this industry.</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>Photographic film, paper, plate and chemical mfg.</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>325992</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>NAICS</x:v>
+      </x:c>
+      <x:c t="str">
         <x:v>0</x:v>
       </x:c>
       <x:c t="str">
@@ -3340,6 +4366,25 @@
         <x:v>EPA</x:v>
       </x:c>
       <x:c t="str">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>GS</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>The synthetic fiber industry is conventionally divided into two types of
+productS, the semi-synthetics or ceUulosics. which are derived from wood pulp, and the true synthetics or non-ceUulosics. made from primary petrochemicals. This scenario addresses the production of each of these fiber types.</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>Synthetic Fiber Manufacturing</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>n.a.</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>n.a.</x:v>
+      </x:c>
+      <x:c t="str">
         <x:v>8</x:v>
       </x:c>
       <x:c t="str">
@@ -3399,6 +4444,24 @@
         <x:v>EPA</x:v>
       </x:c>
       <x:c t="str">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>GS</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>The purpose of this generic scenario was to search available sources of information to obtain data on production, exposure, and releases for CEB to use in the assessment of PMNs. This generic scenario is applicable for any surfactant used in powder or liquid detergents at commercial or Industrial laundry facilities. It covers most (but not all) of the detergent formulation processes and the use of a surfactanVdetergent at both industrial and commercial laundry facilities.</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>Soap and other Detergents and Surface Active Agents and Industrial Launderers</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>2841; 2843; 7218</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>SIC</x:v>
+      </x:c>
+      <x:c t="str">
         <x:v>2</x:v>
       </x:c>
       <x:c t="str">
@@ -3458,6 +4521,27 @@
         <x:v>EPA</x:v>
       </x:c>
       <x:c t="str">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>GS</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>The purpose of this report is to develop a standardized approach that EPA's Chemical Engineering Branch (CEB) can use to estimate potential occupational exposures and environmental releases from new chemicals used in the Metal Products and Machinery (MP&amp;M) industry. This document also presents a detailed discussion of the MP&amp;M industry and the unit operations that are involved.
+Information used to develop the estimation procedures was obtained from the Metal Products and Machinery Effluent Limitations Guidelines Technical Development Document, including sampling data and data submitted by industry to EPA in response to the 1989 and 1996 Metal Products and Machinery Data Collection Portfolios.
+For the purpose of this report, an estimation methodology was developed for two subcategories of the MP&amp;M industry; metal finishing and metal shaping. This division was based on industry experience and data that show a substantial difference in the operations and potential releases from each subcategory.
+Based on the analysis of information and data, reasonable worst-case release and exposure estimations can be made using the methodology and calculations that are discussed in detail in Sections 4 and 5. The calculations are summarized in Tables A-1 and A-2.</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>Aerospace; Aircraft; Electronic Equipment; Hardware; Mobile Industrial Equipment; Ordnance; Stationary Industrial Equipment; Bus and Truck; Household Equipment; Instruments; Motor Vehicle; Office Machine; Precious and Nonprecious Metals; Railroad; Ships and Boats; Printed Wiring Boards; Job Shops; Miscellaneous Metal Products</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>n.a.</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>n.a.</x:v>
+      </x:c>
+      <x:c t="str">
         <x:v>0</x:v>
       </x:c>
       <x:c t="str">
@@ -3517,6 +4601,24 @@
         <x:v>EPA</x:v>
       </x:c>
       <x:c t="str">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>GS</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>This model estimates an environmental release of coating formulation or its chemical components due to coating application inefficiencies during roll and curtain coating operations. The scope of this model is limited to losses from the coating operation due to overall application loss due to transfer inefficiencies. Specifically, this loss represents the fraction of the coating formulation that does not remain on the substrate during the coating process. The generic model is only applicable to estimate releases from the application of the coating and not to releases from other activities at the site (e.g., spills during loading, cleaning, etc.).</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>Coatings</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>n.a.</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>n.a.</x:v>
+      </x:c>
+      <x:c t="str">
         <x:v>0</x:v>
       </x:c>
       <x:c t="str">
@@ -3574,6 +4676,24 @@
       </x:c>
       <x:c t="str">
         <x:v>EPA</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>GS</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>This document presents a standard approach for estimating worker exposures to and environmental releases of non-volatile chemicals used in spray coatings for the metal and wooden furniture manufacturing industry. It does not cover worker exposures or environmental releases from the formulation of the coatings. The scenario covers the application of liquid coatings to furniture via spray coating, and does not cover coatings applied via roll coating or electrostatic application (powder coatings). The formulation of latex/emulsion coatings, roll coating, and electrostatic application are covered under other generic scenarios.</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>Metal household furniture; non-wood office furniture manufacturing; institutional furniture framing; show case, partioning, shelving, and locker manufacturing; non-upholstered wood household furniture mfg.; wood television, radio, and sewing machine cabinet manufacturing; wood office furniture manufacturing; custom architectural woodwork and mill work manufacturing; wood kitchen cabinet and counter top manufacturing</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>337124; 337214; 337127; 337215; 337122; 337129; 337211; 337212; 337110</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>NAICS</x:v>
       </x:c>
       <x:c t="str">
         <x:v>2</x:v>

</xml_diff>